<commit_message>
added longest possible dataseries
</commit_message>
<xml_diff>
--- a/data/inflation_DK_MONAdata.xlsx
+++ b/data/inflation_DK_MONAdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
   <si>
     <t>19841 *Q</t>
   </si>
@@ -576,7 +576,16 @@
     <t>Danmarks Nationalbank</t>
   </si>
   <si>
-    <t>Raw oil price, \$/Barrel</t>
+    <t>Gross Domestic Product (T.tn.Chn.2010DKK), Seasonally adjusted</t>
+  </si>
+  <si>
+    <t>Labor force per thousands, seasonally adjusted, national accounts enployment minus persons on leave plus persons in activation</t>
+  </si>
+  <si>
+    <t>Unemployment rate, seasonally adjusted, unemployed net of persons on leave relative to labor force</t>
+  </si>
+  <si>
+    <t>World, Crude Oil, Brent, Spot, FOB North Sea, ICE, Close, $/Barrel</t>
   </si>
 </sst>
 </file>
@@ -955,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1007,16 +1016,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="6" t="s">
         <v>182</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>168</v>

</xml_diff>